<commit_message>
fix change import file
</commit_message>
<xml_diff>
--- a/public/export/bieumaunhaplieu.xlsx
+++ b/public/export/bieumaunhaplieu.xlsx
@@ -15,33 +15,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
-  <si>
-    <t>123</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+  <si>
+    <t>Bieu mau Test</t>
   </si>
   <si>
     <t>Địa bàn:</t>
   </si>
   <si>
-    <t>Chi Cục Thống Kê</t>
+    <t>Test</t>
   </si>
   <si>
     <t>Khu vực</t>
   </si>
   <si>
-    <t>Toàn tỉnh</t>
+    <t>Chỉ huyện</t>
   </si>
   <si>
     <t>Loại số liệu</t>
   </si>
   <si>
-    <t>KH Năm</t>
+    <t>Tháng</t>
   </si>
   <si>
     <t>Kỳ nhập liệu</t>
   </si>
   <si>
-    <t>Năm</t>
+    <t>Báo cáo năm 2020</t>
   </si>
   <si>
     <t>Năm nhập biểu mẫu</t>
@@ -59,16 +59,22 @@
     <t>Đơn vị</t>
   </si>
   <si>
-    <t>Tỷ lệ chất thải rắn ở đô thị được thu gom</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>Số cơ sở gây ô nhiễm môi trường nghiêm trọng được xử lý  (*)</t>
-  </si>
-  <si>
-    <t>Số khu công nghiệp, khu chế xuất đang hoạt động</t>
+    <t>Chi tiêu cha</t>
+  </si>
+  <si>
+    <t>Bich</t>
+  </si>
+  <si>
+    <t>Chi tieu con</t>
+  </si>
+  <si>
+    <t>Hop</t>
+  </si>
+  <si>
+    <t>Chi tieu test</t>
+  </si>
+  <si>
+    <t>Chi tieu test 5</t>
   </si>
 </sst>
 </file>
@@ -489,10 +495,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:X11"/>
+  <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A8" sqref="A8:C11"/>
+      <selection activeCell="A8" sqref="A8:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -611,7 +617,7 @@
         <v>15</v>
       </c>
       <c r="F8" s="7">
-        <v>6002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:24">
@@ -620,28 +626,40 @@
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F9" s="7">
-        <v>6003</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:24">
       <c r="A10" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F10" s="7">
-        <v>6004</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:24">
-      <c r="A11" s="9"/>
+      <c r="A11" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
+      <c r="C11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>